<commit_message>
EPBDS-10595 Improve @ServiceExtraMethod to use generated beans from the rules. Arrays support is added,
</commit_message>
<xml_diff>
--- a/ITEST/itest.WebService/openl-repository/EPBDS-10595/EPBDS-10595/Main.xlsx
+++ b/ITEST/itest.WebService/openl-repository/EPBDS-10595/EPBDS-10595/Main.xlsx
@@ -1,36 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\demo\openl-demo\user-workspace\DEFAULT\VariationsBug\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\ITEST\itest.WebService\openl-repository\EPBDS-10595\EPBDS-10595\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D808245C-ECC0-4364-984B-DB7534811FB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B99FE23-BD93-444F-B1EA-A45CB5C9877C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2625" yWindow="990" windowWidth="23895" windowHeight="13470" xr2:uid="{FF09DCA3-B6FA-4E8C-88BA-BD4ED29642D4}"/>
+    <workbookView xWindow="7360" yWindow="3660" windowWidth="24340" windowHeight="15820" xr2:uid="{FF09DCA3-B6FA-4E8C-88BA-BD4ED29642D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
   <si>
     <t>Datatype MyDatatype</t>
   </si>
@@ -59,24 +54,29 @@
     <t>a</t>
   </si>
   <si>
-    <t>b</t>
-  </si>
-  <si>
     <t>c</t>
   </si>
   <si>
     <t>SmartRules Double myRule(MyDatatype inputParam)</t>
+  </si>
+  <si>
+    <t>SmartRules Double myRule(MyDatatype[] inputParam, String x)</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>SmartRules Double myRule2(MyDatatype[] inputParam, String x)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1" rgb="000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -109,7 +109,7 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -428,23 +428,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A43C95D-9A70-41BE-91DC-D9A601FA420A}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C9" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C10" t="s">
         <v>1</v>
       </c>
@@ -452,7 +452,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C11" t="s">
         <v>3</v>
       </c>
@@ -460,12 +460,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C15" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C16" t="s">
         <v>5</v>
       </c>
@@ -476,7 +476,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C17" t="s">
         <v>8</v>
       </c>
@@ -487,7 +487,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C18" t="s">
         <v>8</v>
       </c>
@@ -498,14 +498,88 @@
         <v>200</v>
       </c>
     </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D19">
         <v>3</v>
       </c>
       <c r="E19">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="25" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C26" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C27" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="29" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C29" t="s">
+        <v>9</v>
+      </c>
+      <c r="D29">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="35" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C35" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C36" t="s">
+        <v>12</v>
+      </c>
+      <c r="D36" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C37" t="s">
+        <v>8</v>
+      </c>
+      <c r="D37">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C38" t="s">
+        <v>8</v>
+      </c>
+      <c r="D38">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="39" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C39" t="s">
+        <v>9</v>
+      </c>
+      <c r="D39">
         <v>300</v>
       </c>
     </row>

</xml_diff>